<commit_message>
Writing Multiple Data into excel program with Flipkart Scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata.xlsx
+++ b/src/test/resources/Testdata.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project videos\wcsm18\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB9ED0A-5B40-4B3C-8966-C59B4F428423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A433EDA3-4009-415D-8C69-EA58A5610779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C517A452-2B37-4394-A64B-64B2B23F9A33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C517A452-2B37-4394-A64B-64B2B23F9A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MobilesPrices" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>username</t>
   </si>
@@ -54,13 +55,114 @@
   </si>
   <si>
     <t>656876988</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy F13 (Sunrise Copper, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹9,499</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 (White, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹35,990</t>
+  </si>
+  <si>
+    <t>IAIR D41</t>
+  </si>
+  <si>
+    <t>₹1,319</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy F13 (Nightsky Green, 64 GB)</t>
+  </si>
+  <si>
+    <t>REDMI 10 (Midnight Black, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹8,549</t>
+  </si>
+  <si>
+    <t>REDMI 10 (Caribbean Green, 64 GB)</t>
+  </si>
+  <si>
+    <t>realme C30 (Lake Blue, 32 GB)</t>
+  </si>
+  <si>
+    <t>₹5,699</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 13 (Midnight, 128 GB)</t>
+  </si>
+  <si>
+    <t>₹59,990</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 13 (Starlight, 128 GB)</t>
+  </si>
+  <si>
+    <t>realme C30 (Denim Black, 32 GB)</t>
+  </si>
+  <si>
+    <t>realme C30 (Bamboo Green, 32 GB)</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 13 (Green, 128 GB)</t>
+  </si>
+  <si>
+    <t>Infinix HOT 12 Play (Horizon Blue, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹8,199</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 (Black, 64 GB)</t>
+  </si>
+  <si>
+    <t>POCO C31 (Royal Blue, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹7,749</t>
+  </si>
+  <si>
+    <t>APPLE iPhone 11 (White, 128 GB)</t>
+  </si>
+  <si>
+    <t>₹42,990</t>
+  </si>
+  <si>
+    <t>realme C33 (Night Sea, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹9,999</t>
+  </si>
+  <si>
+    <t>realme C33 (Aqua Blue, 32 GB)</t>
+  </si>
+  <si>
+    <t>₹8,999</t>
+  </si>
+  <si>
+    <t>realme C33 (Night Sea, 32 GB)</t>
+  </si>
+  <si>
+    <t>realme C33 (Sandy Gold, 32 GB)</t>
+  </si>
+  <si>
+    <t>realme C33 (Sandy Gold, 64 GB)</t>
+  </si>
+  <si>
+    <t>Infinix HOT 12 Play (Racing Black, 64 GB)</t>
+  </si>
+  <si>
+    <t>Infinix HOT 12 Play (Champagne Gold, 64 GB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,15 +511,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EC9E1C-D1E6-46A7-A3AB-1E5FDB46D867}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="18.44140625"/>
-    <col min="2" max="2" customWidth="true" style="1" width="34.44140625"/>
-    <col min="3" max="16384" style="1" width="8.88671875"/>
+    <col min="1" max="1" width="18.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -452,12 +554,213 @@
         <v>345678</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{109B1749-F0F4-48EE-86BD-B130A7BB117E}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="77.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>